<commit_message>
save valor con su funcion
</commit_message>
<xml_diff>
--- a/TRAMA-PRUEBAS.xlsx
+++ b/TRAMA-PRUEBAS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">NRO CREDITO</t>
   </si>
@@ -50,6 +50,36 @@
   </si>
   <si>
     <t xml:space="preserve">SOLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validarnumero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valoresposibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validarcaracteres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valoresposilbes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitudadmaxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor – string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor string, valoresPosibles [] string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor – string, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">texto string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor – string, longitud int</t>
   </si>
 </sst>
 </file>
@@ -257,10 +287,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.38"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -315,13 +353,30 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3"/>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -333,13 +388,30 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3"/>
+      <c r="C9" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>

</xml_diff>